<commit_message>
Update no UseCase registaStock
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/RegistarChegadaDeStock.xlsx
+++ b/diagramas/UseCases/RegistarChegadaDeStock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/DSS/Configura-Facil/diagramas/UseCases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BCD91E-2AA0-EA44-AC4D-FBC26EAE4494}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E5326-DF34-9A47-A6AE-09EE7E33C5C6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Actor input</t>
   </si>
@@ -58,19 +58,10 @@
     <t>Stock registado e categorizado</t>
   </si>
   <si>
-    <t>1. Apresenta a chegada de stock</t>
-  </si>
-  <si>
-    <t>2. Categoriza o stock</t>
-  </si>
-  <si>
-    <t>Cenário alternativo 1 [não existe a categoria correspondente a uma determinada peça] (passo 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1 Cria uma categoria nova </t>
-  </si>
-  <si>
-    <t>2.2 Regrassar a 2</t>
+    <t>2. Processa o novo stock</t>
+  </si>
+  <si>
+    <t>1.Regista o stock que chegou ao sistema</t>
   </si>
 </sst>
 </file>
@@ -107,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -177,19 +168,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -246,43 +224,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -291,31 +232,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,10 +257,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -647,9 +577,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -657,134 +587,112 @@
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="1" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
     <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B17:B19"/>
+  <mergeCells count="5">
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>

<commit_message>
Revisão do Registar Stock
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/RegistarChegadaDeStock.xlsx
+++ b/diagramas/UseCases/RegistarChegadaDeStock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E5326-DF34-9A47-A6AE-09EE7E33C5C6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92FD582-EF06-4C91-A9F9-23AF54F5BB01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -58,10 +58,10 @@
     <t>Stock registado e categorizado</t>
   </si>
   <si>
-    <t>2. Processa o novo stock</t>
-  </si>
-  <si>
-    <t>1.Regista o stock que chegou ao sistema</t>
+    <t>1. Categoriza e quantifica stock que chegou</t>
+  </si>
+  <si>
+    <t>2. Adiciona stock ao sistema</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -262,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,20 +582,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
     <col min="3" max="3" width="41.5" customWidth="1"/>
     <col min="4" max="4" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
@@ -601,7 +604,7 @@
       </c>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -610,14 +613,14 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -626,7 +629,7 @@
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
@@ -637,56 +640,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13"/>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="13"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="13"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="13"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13"/>
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
Adicionados os .pngs dos diagramas
E corrigidas algumas formatações dos use cases
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/RegistarChegadaDeStock.xlsx
+++ b/diagramas/UseCases/RegistarChegadaDeStock.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92FD582-EF06-4C91-A9F9-23AF54F5BB01}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB97A2C6-229D-47F0-8F0D-7509C7604FC8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -245,6 +245,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,9 +265,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -599,38 +599,38 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -641,58 +641,23 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="13"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="13"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="13"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="13"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="13"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="13"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="13"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -700,7 +665,7 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>